<commit_message>
Remove unused QR PDFs and update project structure
Deleted three PDF files from wwwroot/qr and removed the corresponding folder references from the project file. Updated Visual Studio and build metadata files to reflect the new project structure and document layout. Also updated Excel templates in wwwroot/templates.
</commit_message>
<xml_diff>
--- a/apps/MediaService/MediaService/wwwroot/templates/IT_BBBG_Template.xlsx
+++ b/apps/MediaService/MediaService/wwwroot/templates/IT_BBBG_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\vcvapp\apps\MediaService\MediaService\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189228F4-0D60-4FF6-BEE5-17A6761989CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9940FA9-E90F-4E21-8B3F-1FB5CA5250AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{774C9390-FF90-4673-8DC0-539F23F1EC8A}"/>
   </bookViews>
@@ -101,8 +101,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">NO.
-</t>
+      <t xml:space="preserve">                                                  Ngày/ </t>
     </r>
     <r>
       <rPr>
@@ -112,13 +111,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>STT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Asset, Equipment name
-</t>
+      <t>Date:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Assignment ID/ </t>
     </r>
     <r>
       <rPr>
@@ -128,13 +129,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Tên tài sản, công cụ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Unit
-</t>
+      <t>Mã bàn giao</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Receiver/ </t>
     </r>
     <r>
       <rPr>
@@ -144,12 +153,141 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Người nhận bàn giao:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Deliverer/ </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Người bàn giao: </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rationale for handover/ </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lý do bàn giao: </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Together, we hand over assets and tools as follows:/ </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cùng bàn giao tài sản, công cụ với nội dung như sau:</t>
+    </r>
+  </si>
+  <si>
+    <t>The recipient of the handover certifies that they have received the complete quantity and the correct model as specified/</t>
+  </si>
+  <si>
+    <t>Người nhận bàn giao cam kết rằng đã nhận đầy đủ số lượng và đúng mẫu mã.</t>
+  </si>
+  <si>
+    <t>The recipient of the handover is obligated to properly maintain the assets. Should any loss or damage occur, full compensation for the asset's value is required/</t>
+  </si>
+  <si>
+    <t>DELIVERER</t>
+  </si>
+  <si>
+    <t>RECEIVER</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NO.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>STT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Asset, Equipment name
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tên tài sản, công cụ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Equipment and Asset ID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mã tài sản, công cụ </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unit
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Đơn vị tính</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="18"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -159,6 +297,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <i/>
         <sz val="18"/>
         <rFont val="Calibri"/>
@@ -169,145 +308,12 @@
 Số lượng</t>
     </r>
   </si>
-  <si>
-    <r>
-      <t xml:space="preserve">                                                  Ngày/ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Date:</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Assignment ID/ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mã bàn giao</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Receiver/ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Người nhận bàn giao:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Deliverer/ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Người bàn giao: </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rationale for handover/ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Lý do bàn giao: </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Together, we hand over assets and tools as follows:/ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cùng bàn giao tài sản, công cụ với nội dung như sau:</t>
-    </r>
-  </si>
-  <si>
-    <t>The recipient of the handover certifies that they have received the complete quantity and the correct model as specified/</t>
-  </si>
-  <si>
-    <t>Người nhận bàn giao cam kết rằng đã nhận đầy đủ số lượng và đúng mẫu mã.</t>
-  </si>
-  <si>
-    <t>The recipient of the handover is obligated to properly maintain the assets. Should any loss or damage occur, full compensation for the asset's value is required/</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Equipment and Asset ID
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mã tài sản, công cụ </t>
-    </r>
-  </si>
-  <si>
-    <t>DELIVERER</t>
-  </si>
-  <si>
-    <t>RECEIVER</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +354,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="18"/>
       <name val="Calibri"/>
@@ -427,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -450,9 +471,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -480,6 +498,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -489,23 +516,23 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -882,51 +909,51 @@
   </sheetPr>
   <dimension ref="A4:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="56.42578125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="35" style="13" customWidth="1"/>
-    <col min="9" max="9" width="14" style="13" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="13"/>
+    <col min="1" max="1" width="10.140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="56.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="35" style="12" customWidth="1"/>
+    <col min="9" max="9" width="14" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="15"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="15"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -937,7 +964,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="15"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -948,21 +975,21 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="15"/>
+      <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -974,7 +1001,7 @@
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1020,7 +1047,7 @@
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="5"/>
@@ -1066,7 +1093,7 @@
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1078,7 +1105,7 @@
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1099,228 +1126,228 @@
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="7" t="s">
+      <c r="A23" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>14</v>
+      <c r="G23" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
@@ -1334,7 +1361,7 @@
     </row>
     <row r="45" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1346,7 +1373,7 @@
     </row>
     <row r="46" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1358,7 +1385,7 @@
     </row>
     <row r="47" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1369,7 +1396,7 @@
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B48" s="2"/>
@@ -1391,10 +1418,10 @@
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B50" s="22"/>
+      <c r="A50" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="19"/>
       <c r="C50" s="4"/>
       <c r="D50" s="2"/>
       <c r="E50" s="3"/>
@@ -1418,45 +1445,45 @@
     </row>
     <row r="52" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B52" s="25"/>
       <c r="C52" s="25"/>
       <c r="D52" s="25"/>
       <c r="E52" s="3"/>
       <c r="F52" s="25" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G52" s="25"/>
       <c r="H52" s="25"/>
     </row>
     <row r="53" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="26" t="s">
+      <c r="A53" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="26"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="26" t="s">
+      <c r="F53" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G53" s="26"/>
-      <c r="H53" s="26"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
     </row>
     <row r="54" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="s">
+      <c r="A54" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="26" t="s">
+      <c r="F54" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G54" s="26"/>
-      <c r="H54" s="26"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
     </row>
     <row r="55" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
@@ -1499,14 +1526,14 @@
       <c r="H58" s="2"/>
     </row>
     <row r="59" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="25"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
       <c r="E59" s="3"/>
       <c r="F59" s="2"/>
-      <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
     </row>
     <row r="60" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
@@ -1519,16 +1546,15 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
@@ -1545,15 +1571,16 @@
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>